<commit_message>
Add tailor-made input files
</commit_message>
<xml_diff>
--- a/optimization model/data/input-values.xlsx
+++ b/optimization model/data/input-values.xlsx
@@ -174,7 +174,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -188,6 +188,7 @@
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Komma" xfId="1" builtinId="3"/>
@@ -496,7 +497,7 @@
   <dimension ref="A1:G145"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -507,7 +508,7 @@
     <col min="4" max="4" width="51.21875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.77734375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
@@ -645,7 +646,7 @@
         <v>2025</v>
       </c>
       <c r="G6" s="10">
-        <v>900</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
@@ -782,7 +783,7 @@
       <c r="G17" s="2"/>
     </row>
     <row r="18" spans="7:7" x14ac:dyDescent="0.3">
-      <c r="G18" s="2"/>
+      <c r="G18" s="11"/>
     </row>
     <row r="19" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G19" s="2"/>

</xml_diff>

<commit_message>
Add sensitivity analysis (text, code, etc.)
</commit_message>
<xml_diff>
--- a/optimization model/data/input-values.xlsx
+++ b/optimization model/data/input-values.xlsx
@@ -503,7 +503,7 @@
   <dimension ref="A1:L145"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -781,103 +781,27 @@
       <c r="G14" s="2"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="G15" s="2">
-        <v>5</v>
-      </c>
-      <c r="H15">
-        <f>G15*30*$G$6</f>
-        <v>150000</v>
-      </c>
-      <c r="I15" s="12">
-        <f>30*$G$7</f>
-        <v>45000</v>
-      </c>
-      <c r="J15">
-        <f>SUM(H15:I15)</f>
-        <v>195000</v>
-      </c>
-      <c r="K15">
-        <v>0</v>
-      </c>
-      <c r="L15" s="14">
-        <f>K15/J15</f>
-        <v>0</v>
-      </c>
+      <c r="G15" s="2"/>
+      <c r="I15" s="12"/>
+      <c r="L15" s="14"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="G16" s="2">
-        <f>0.9*G15</f>
-        <v>4.5</v>
-      </c>
-      <c r="H16">
-        <f t="shared" ref="H16:H18" si="0">G16*30*$G$6</f>
-        <v>135000</v>
-      </c>
-      <c r="I16" s="12">
-        <f t="shared" ref="I16:I18" si="1">30*$G$7</f>
-        <v>45000</v>
-      </c>
-      <c r="J16">
-        <f t="shared" ref="J16:J18" si="2">SUM(H16:I16)</f>
-        <v>180000</v>
-      </c>
-      <c r="K16" s="13">
-        <v>64390.92</v>
-      </c>
-      <c r="L16" s="14">
-        <f t="shared" ref="L16:L18" si="3">K16/J16</f>
-        <v>0.35772733333333334</v>
-      </c>
+      <c r="G16" s="2"/>
+      <c r="I16" s="12"/>
+      <c r="K16" s="13"/>
+      <c r="L16" s="14"/>
     </row>
     <row r="17" spans="7:12" x14ac:dyDescent="0.3">
-      <c r="G17" s="2">
-        <f>0.8*G15</f>
-        <v>4</v>
-      </c>
-      <c r="H17">
-        <f t="shared" si="0"/>
-        <v>120000</v>
-      </c>
-      <c r="I17" s="12">
-        <f t="shared" si="1"/>
-        <v>45000</v>
-      </c>
-      <c r="J17">
-        <f t="shared" si="2"/>
-        <v>165000</v>
-      </c>
-      <c r="K17" s="13">
-        <v>4144.25</v>
-      </c>
-      <c r="L17" s="14">
-        <f t="shared" si="3"/>
-        <v>2.5116666666666666E-2</v>
-      </c>
+      <c r="G17" s="2"/>
+      <c r="I17" s="12"/>
+      <c r="K17" s="13"/>
+      <c r="L17" s="14"/>
     </row>
     <row r="18" spans="7:12" x14ac:dyDescent="0.3">
-      <c r="G18" s="11">
-        <f>0.7*G15</f>
-        <v>3.5</v>
-      </c>
-      <c r="H18">
-        <f t="shared" si="0"/>
-        <v>105000</v>
-      </c>
-      <c r="I18" s="12">
-        <f t="shared" si="1"/>
-        <v>45000</v>
-      </c>
-      <c r="J18">
-        <f t="shared" si="2"/>
-        <v>150000</v>
-      </c>
-      <c r="K18" s="13">
-        <v>7455.72</v>
-      </c>
-      <c r="L18" s="14">
-        <f t="shared" si="3"/>
-        <v>4.97048E-2</v>
-      </c>
+      <c r="G18" s="11"/>
+      <c r="I18" s="12"/>
+      <c r="K18" s="13"/>
+      <c r="L18" s="14"/>
     </row>
     <row r="19" spans="7:12" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G19" s="2"/>

</xml_diff>

<commit_message>
Minor edits in the model
</commit_message>
<xml_diff>
--- a/optimization model/data/input-values.xlsx
+++ b/optimization model/data/input-values.xlsx
@@ -503,7 +503,7 @@
   <dimension ref="A1:L145"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -607,7 +607,7 @@
         <v>2025</v>
       </c>
       <c r="G4" s="8">
-        <v>0.1</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">

</xml_diff>